<commit_message>
add rows for jjuly-2020
</commit_message>
<xml_diff>
--- a/data/11/weather_diff.xlsx
+++ b/data/11/weather_diff.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seungmi/workspace/studying/bigcon_mmmz/master/data/11/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37744D96-D136-FA43-8732-5672695F2176}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="860" yWindow="20" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -28,11 +34,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -96,6 +102,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -142,7 +156,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -174,9 +188,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -208,6 +240,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -383,14 +433,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D366"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D367"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A355" workbookViewId="0">
+      <selection activeCell="G366" sqref="G366"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -401,7 +456,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -415,7 +470,7 @@
         <v>7.6</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -429,7 +484,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -443,7 +498,7 @@
         <v>11.6</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -457,7 +512,7 @@
         <v>10.3</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -471,7 +526,7 @@
         <v>6.6</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -485,7 +540,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -496,10 +551,10 @@
         <v>0</v>
       </c>
       <c r="D8">
-        <v>9.300000000000001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+        <v>9.3000000000000007</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -513,7 +568,7 @@
         <v>7.7</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -527,7 +582,7 @@
         <v>10.7</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -541,7 +596,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -552,10 +607,10 @@
         <v>0</v>
       </c>
       <c r="D12">
-        <v>7.600000000000001</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
+        <v>7.6000000000000014</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -569,7 +624,7 @@
         <v>8.6</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -583,7 +638,7 @@
         <v>10.6</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -594,10 +649,10 @@
         <v>0</v>
       </c>
       <c r="D15">
-        <v>7.699999999999999</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
+        <v>7.6999999999999993</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -608,10 +663,10 @@
         <v>0</v>
       </c>
       <c r="D16">
-        <v>9.800000000000001</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
+        <v>9.8000000000000007</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -625,7 +680,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -639,7 +694,7 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -653,7 +708,7 @@
         <v>11.3</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -667,7 +722,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -681,7 +736,7 @@
         <v>9.5</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -695,7 +750,7 @@
         <v>10.9</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -709,7 +764,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -723,7 +778,7 @@
         <v>7.8</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -737,7 +792,7 @@
         <v>11.1</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -751,7 +806,7 @@
         <v>6.4</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -765,7 +820,7 @@
         <v>8.9</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -779,7 +834,7 @@
         <v>11.7</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -793,7 +848,7 @@
         <v>6.9</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -807,7 +862,7 @@
         <v>12.6</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -818,10 +873,10 @@
         <v>0</v>
       </c>
       <c r="D31">
-        <v>9.399999999999999</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
+        <v>9.3999999999999986</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -835,7 +890,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -846,10 +901,10 @@
         <v>0</v>
       </c>
       <c r="D33">
-        <v>10.2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
+        <v>10.199999999999999</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -860,10 +915,10 @@
         <v>0</v>
       </c>
       <c r="D34">
-        <v>9.300000000000001</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4">
+        <v>9.3000000000000007</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -877,7 +932,7 @@
         <v>2.9</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -891,7 +946,7 @@
         <v>6.3</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -905,7 +960,7 @@
         <v>13.7</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -916,10 +971,10 @@
         <v>0</v>
       </c>
       <c r="D38">
-        <v>9.200000000000001</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4">
+        <v>9.2000000000000011</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -933,7 +988,7 @@
         <v>14.5</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -944,10 +999,10 @@
         <v>0</v>
       </c>
       <c r="D40">
-        <v>8.899999999999999</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4">
+        <v>8.8999999999999986</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -958,10 +1013,10 @@
         <v>0</v>
       </c>
       <c r="D41">
-        <v>6.699999999999999</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4">
+        <v>6.6999999999999993</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -972,10 +1027,10 @@
         <v>0</v>
       </c>
       <c r="D42">
-        <v>7.199999999999999</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4">
+        <v>7.1999999999999993</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -989,7 +1044,7 @@
         <v>9.5</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -1003,7 +1058,7 @@
         <v>7.8</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -1014,10 +1069,10 @@
         <v>0</v>
       </c>
       <c r="D45">
-        <v>8.199999999999999</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4">
+        <v>8.1999999999999993</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -1031,7 +1086,7 @@
         <v>12.2</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -1045,7 +1100,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -1059,7 +1114,7 @@
         <v>6.6</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -1073,7 +1128,7 @@
         <v>11.4</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -1087,7 +1142,7 @@
         <v>10.6</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -1101,7 +1156,7 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -1112,10 +1167,10 @@
         <v>0</v>
       </c>
       <c r="D52">
-        <v>4.6</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -1129,7 +1184,7 @@
         <v>11.6</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -1143,7 +1198,7 @@
         <v>12.4</v>
       </c>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -1157,7 +1212,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -1171,7 +1226,7 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -1182,10 +1237,10 @@
         <v>0</v>
       </c>
       <c r="D57">
-        <v>8.899999999999999</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4">
+        <v>8.8999999999999986</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -1199,7 +1254,7 @@
         <v>13.5</v>
       </c>
     </row>
-    <row r="59" spans="1:4">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -1210,10 +1265,10 @@
         <v>0</v>
       </c>
       <c r="D59">
-        <v>9.300000000000001</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4">
+        <v>9.3000000000000007</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -1227,7 +1282,7 @@
         <v>10.8</v>
       </c>
     </row>
-    <row r="61" spans="1:4">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -1241,7 +1296,7 @@
         <v>11.8</v>
       </c>
     </row>
-    <row r="62" spans="1:4">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -1255,7 +1310,7 @@
         <v>13.4</v>
       </c>
     </row>
-    <row r="63" spans="1:4">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -1269,7 +1324,7 @@
         <v>13.6</v>
       </c>
     </row>
-    <row r="64" spans="1:4">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -1283,7 +1338,7 @@
         <v>11.3</v>
       </c>
     </row>
-    <row r="65" spans="1:4">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -1294,10 +1349,10 @@
         <v>0</v>
       </c>
       <c r="D65">
-        <v>7.300000000000001</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4">
+        <v>7.3000000000000007</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -1311,7 +1366,7 @@
         <v>6.7</v>
       </c>
     </row>
-    <row r="67" spans="1:4">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -1325,7 +1380,7 @@
         <v>9.6</v>
       </c>
     </row>
-    <row r="68" spans="1:4">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -1339,7 +1394,7 @@
         <v>12.8</v>
       </c>
     </row>
-    <row r="69" spans="1:4">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -1353,7 +1408,7 @@
         <v>15.3</v>
       </c>
     </row>
-    <row r="70" spans="1:4">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -1364,10 +1419,10 @@
         <v>0</v>
       </c>
       <c r="D70">
-        <v>8.600000000000001</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4">
+        <v>8.6000000000000014</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -1381,7 +1436,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="72" spans="1:4">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -1392,10 +1447,10 @@
         <v>0</v>
       </c>
       <c r="D72">
-        <v>8.200000000000001</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4">
+        <v>8.2000000000000011</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -1409,7 +1464,7 @@
         <v>8.9</v>
       </c>
     </row>
-    <row r="74" spans="1:4">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -1423,7 +1478,7 @@
         <v>11.7</v>
       </c>
     </row>
-    <row r="75" spans="1:4">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -1434,10 +1489,10 @@
         <v>0</v>
       </c>
       <c r="D75">
-        <v>9.700000000000001</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4">
+        <v>9.7000000000000011</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>74</v>
       </c>
@@ -1451,7 +1506,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="77" spans="1:4">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>75</v>
       </c>
@@ -1462,10 +1517,10 @@
         <v>0</v>
       </c>
       <c r="D77">
-        <v>9.800000000000001</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4">
+        <v>9.8000000000000007</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>76</v>
       </c>
@@ -1479,7 +1534,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="79" spans="1:4">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>77</v>
       </c>
@@ -1493,7 +1548,7 @@
         <v>13.3</v>
       </c>
     </row>
-    <row r="80" spans="1:4">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>78</v>
       </c>
@@ -1507,7 +1562,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="81" spans="1:4">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>79</v>
       </c>
@@ -1518,10 +1573,10 @@
         <v>0</v>
       </c>
       <c r="D81">
-        <v>9.199999999999999</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4">
+        <v>9.1999999999999993</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -1535,7 +1590,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="83" spans="1:4">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
         <v>81</v>
       </c>
@@ -1549,7 +1604,7 @@
         <v>8.6</v>
       </c>
     </row>
-    <row r="84" spans="1:4">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
         <v>82</v>
       </c>
@@ -1563,7 +1618,7 @@
         <v>10.5</v>
       </c>
     </row>
-    <row r="85" spans="1:4">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
         <v>83</v>
       </c>
@@ -1577,7 +1632,7 @@
         <v>8.6</v>
       </c>
     </row>
-    <row r="86" spans="1:4">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
         <v>84</v>
       </c>
@@ -1588,10 +1643,10 @@
         <v>0</v>
       </c>
       <c r="D86">
-        <v>10.2</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4">
+        <v>10.199999999999999</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
         <v>85</v>
       </c>
@@ -1602,10 +1657,10 @@
         <v>0</v>
       </c>
       <c r="D87">
-        <v>7.299999999999999</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4">
+        <v>7.2999999999999989</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
         <v>86</v>
       </c>
@@ -1619,7 +1674,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="89" spans="1:4">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
         <v>87</v>
       </c>
@@ -1633,7 +1688,7 @@
         <v>9.6</v>
       </c>
     </row>
-    <row r="90" spans="1:4">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
         <v>88</v>
       </c>
@@ -1644,10 +1699,10 @@
         <v>0</v>
       </c>
       <c r="D90">
-        <v>4.9</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4">
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
         <v>89</v>
       </c>
@@ -1658,10 +1713,10 @@
         <v>0</v>
       </c>
       <c r="D91">
-        <v>5.800000000000001</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4">
+        <v>5.8000000000000007</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
         <v>90</v>
       </c>
@@ -1675,7 +1730,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="93" spans="1:4">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
         <v>91</v>
       </c>
@@ -1689,7 +1744,7 @@
         <v>11.7</v>
       </c>
     </row>
-    <row r="94" spans="1:4">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
         <v>92</v>
       </c>
@@ -1703,7 +1758,7 @@
         <v>11.7</v>
       </c>
     </row>
-    <row r="95" spans="1:4">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" s="1">
         <v>93</v>
       </c>
@@ -1717,7 +1772,7 @@
         <v>12.7</v>
       </c>
     </row>
-    <row r="96" spans="1:4">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
         <v>94</v>
       </c>
@@ -1728,10 +1783,10 @@
         <v>0</v>
       </c>
       <c r="D96">
-        <v>10.2</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4">
+        <v>10.199999999999999</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" s="1">
         <v>95</v>
       </c>
@@ -1742,10 +1797,10 @@
         <v>0</v>
       </c>
       <c r="D97">
-        <v>6.299999999999999</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4">
+        <v>6.2999999999999989</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" s="1">
         <v>96</v>
       </c>
@@ -1759,7 +1814,7 @@
         <v>14.7</v>
       </c>
     </row>
-    <row r="99" spans="1:4">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" s="1">
         <v>97</v>
       </c>
@@ -1773,7 +1828,7 @@
         <v>9.6</v>
       </c>
     </row>
-    <row r="100" spans="1:4">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" s="1">
         <v>98</v>
       </c>
@@ -1784,10 +1839,10 @@
         <v>1</v>
       </c>
       <c r="D100">
-        <v>9.199999999999999</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4">
+        <v>9.1999999999999993</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" s="1">
         <v>99</v>
       </c>
@@ -1798,10 +1853,10 @@
         <v>1</v>
       </c>
       <c r="D101">
-        <v>5.499999999999999</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4">
+        <v>5.4999999999999991</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" s="1">
         <v>100</v>
       </c>
@@ -1815,7 +1870,7 @@
         <v>11.4</v>
       </c>
     </row>
-    <row r="103" spans="1:4">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" s="1">
         <v>101</v>
       </c>
@@ -1829,7 +1884,7 @@
         <v>12.9</v>
       </c>
     </row>
-    <row r="104" spans="1:4">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" s="1">
         <v>102</v>
       </c>
@@ -1843,7 +1898,7 @@
         <v>11.7</v>
       </c>
     </row>
-    <row r="105" spans="1:4">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" s="1">
         <v>103</v>
       </c>
@@ -1854,10 +1909,10 @@
         <v>0</v>
       </c>
       <c r="D105">
-        <v>6.699999999999999</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4">
+        <v>6.6999999999999993</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" s="1">
         <v>104</v>
       </c>
@@ -1871,7 +1926,7 @@
         <v>14.2</v>
       </c>
     </row>
-    <row r="107" spans="1:4">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" s="1">
         <v>105</v>
       </c>
@@ -1885,7 +1940,7 @@
         <v>15.8</v>
       </c>
     </row>
-    <row r="108" spans="1:4">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" s="1">
         <v>106</v>
       </c>
@@ -1899,7 +1954,7 @@
         <v>12.7</v>
       </c>
     </row>
-    <row r="109" spans="1:4">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" s="1">
         <v>107</v>
       </c>
@@ -1910,10 +1965,10 @@
         <v>0</v>
       </c>
       <c r="D109">
-        <v>5.799999999999999</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4">
+        <v>5.7999999999999989</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" s="1">
         <v>108</v>
       </c>
@@ -1927,7 +1982,7 @@
         <v>10.1</v>
       </c>
     </row>
-    <row r="111" spans="1:4">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" s="1">
         <v>109</v>
       </c>
@@ -1938,10 +1993,10 @@
         <v>0</v>
       </c>
       <c r="D111">
-        <v>9.400000000000002</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4">
+        <v>9.4000000000000021</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" s="1">
         <v>110</v>
       </c>
@@ -1955,7 +2010,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="113" spans="1:4">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" s="1">
         <v>111</v>
       </c>
@@ -1969,7 +2024,7 @@
         <v>17.5</v>
       </c>
     </row>
-    <row r="114" spans="1:4">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" s="1">
         <v>112</v>
       </c>
@@ -1980,10 +2035,10 @@
         <v>0</v>
       </c>
       <c r="D114">
-        <v>10.2</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4">
+        <v>10.199999999999999</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" s="1">
         <v>113</v>
       </c>
@@ -1997,7 +2052,7 @@
         <v>10.1</v>
       </c>
     </row>
-    <row r="116" spans="1:4">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" s="1">
         <v>114</v>
       </c>
@@ -2008,10 +2063,10 @@
         <v>1</v>
       </c>
       <c r="D116">
-        <v>7.799999999999999</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4">
+        <v>7.7999999999999989</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" s="1">
         <v>115</v>
       </c>
@@ -2025,7 +2080,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="118" spans="1:4">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" s="1">
         <v>116</v>
       </c>
@@ -2039,7 +2094,7 @@
         <v>14.1</v>
       </c>
     </row>
-    <row r="119" spans="1:4">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119" s="1">
         <v>117</v>
       </c>
@@ -2050,10 +2105,10 @@
         <v>0</v>
       </c>
       <c r="D119">
-        <v>6.700000000000001</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4">
+        <v>6.7000000000000011</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" s="1">
         <v>118</v>
       </c>
@@ -2067,7 +2122,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="121" spans="1:4">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121" s="1">
         <v>119</v>
       </c>
@@ -2081,7 +2136,7 @@
         <v>13.5</v>
       </c>
     </row>
-    <row r="122" spans="1:4">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122" s="1">
         <v>120</v>
       </c>
@@ -2095,7 +2150,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="123" spans="1:4">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123" s="1">
         <v>121</v>
       </c>
@@ -2109,7 +2164,7 @@
         <v>14.7</v>
       </c>
     </row>
-    <row r="124" spans="1:4">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124" s="1">
         <v>122</v>
       </c>
@@ -2123,7 +2178,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="125" spans="1:4">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125" s="1">
         <v>123</v>
       </c>
@@ -2137,7 +2192,7 @@
         <v>15.4</v>
       </c>
     </row>
-    <row r="126" spans="1:4">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A126" s="1">
         <v>124</v>
       </c>
@@ -2151,7 +2206,7 @@
         <v>12.9</v>
       </c>
     </row>
-    <row r="127" spans="1:4">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A127" s="1">
         <v>125</v>
       </c>
@@ -2165,7 +2220,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="128" spans="1:4">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128" s="1">
         <v>126</v>
       </c>
@@ -2179,7 +2234,7 @@
         <v>13.5</v>
       </c>
     </row>
-    <row r="129" spans="1:4">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A129" s="1">
         <v>127</v>
       </c>
@@ -2193,7 +2248,7 @@
         <v>11.2</v>
       </c>
     </row>
-    <row r="130" spans="1:4">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A130" s="1">
         <v>128</v>
       </c>
@@ -2207,7 +2262,7 @@
         <v>11.2</v>
       </c>
     </row>
-    <row r="131" spans="1:4">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A131" s="1">
         <v>129</v>
       </c>
@@ -2221,7 +2276,7 @@
         <v>16.5</v>
       </c>
     </row>
-    <row r="132" spans="1:4">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A132" s="1">
         <v>130</v>
       </c>
@@ -2235,7 +2290,7 @@
         <v>15.1</v>
       </c>
     </row>
-    <row r="133" spans="1:4">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A133" s="1">
         <v>131</v>
       </c>
@@ -2249,7 +2304,7 @@
         <v>14.2</v>
       </c>
     </row>
-    <row r="134" spans="1:4">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A134" s="1">
         <v>132</v>
       </c>
@@ -2260,10 +2315,10 @@
         <v>0</v>
       </c>
       <c r="D134">
-        <v>7.300000000000001</v>
-      </c>
-    </row>
-    <row r="135" spans="1:4">
+        <v>7.3000000000000007</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A135" s="1">
         <v>133</v>
       </c>
@@ -2277,7 +2332,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="136" spans="1:4">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A136" s="1">
         <v>134</v>
       </c>
@@ -2291,7 +2346,7 @@
         <v>13.2</v>
       </c>
     </row>
-    <row r="137" spans="1:4">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A137" s="1">
         <v>135</v>
       </c>
@@ -2305,7 +2360,7 @@
         <v>13.3</v>
       </c>
     </row>
-    <row r="138" spans="1:4">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A138" s="1">
         <v>136</v>
       </c>
@@ -2319,7 +2374,7 @@
         <v>10.7</v>
       </c>
     </row>
-    <row r="139" spans="1:4">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A139" s="1">
         <v>137</v>
       </c>
@@ -2330,10 +2385,10 @@
         <v>0</v>
       </c>
       <c r="D139">
-        <v>6.799999999999997</v>
-      </c>
-    </row>
-    <row r="140" spans="1:4">
+        <v>6.7999999999999972</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A140" s="1">
         <v>138</v>
       </c>
@@ -2344,10 +2399,10 @@
         <v>1</v>
       </c>
       <c r="D140">
-        <v>3.700000000000003</v>
-      </c>
-    </row>
-    <row r="141" spans="1:4">
+        <v>3.7000000000000028</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A141" s="1">
         <v>139</v>
       </c>
@@ -2358,10 +2413,10 @@
         <v>1</v>
       </c>
       <c r="D141">
-        <v>7.199999999999999</v>
-      </c>
-    </row>
-    <row r="142" spans="1:4">
+        <v>7.1999999999999993</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A142" s="1">
         <v>140</v>
       </c>
@@ -2375,7 +2430,7 @@
         <v>12.1</v>
       </c>
     </row>
-    <row r="143" spans="1:4">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A143" s="1">
         <v>141</v>
       </c>
@@ -2389,7 +2444,7 @@
         <v>14.2</v>
       </c>
     </row>
-    <row r="144" spans="1:4">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A144" s="1">
         <v>142</v>
       </c>
@@ -2403,7 +2458,7 @@
         <v>14.2</v>
       </c>
     </row>
-    <row r="145" spans="1:4">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A145" s="1">
         <v>143</v>
       </c>
@@ -2417,7 +2472,7 @@
         <v>17.2</v>
       </c>
     </row>
-    <row r="146" spans="1:4">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A146" s="1">
         <v>144</v>
       </c>
@@ -2428,10 +2483,10 @@
         <v>0</v>
       </c>
       <c r="D146">
-        <v>10.2</v>
-      </c>
-    </row>
-    <row r="147" spans="1:4">
+        <v>10.199999999999999</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A147" s="1">
         <v>145</v>
       </c>
@@ -2445,7 +2500,7 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="148" spans="1:4">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A148" s="1">
         <v>146</v>
       </c>
@@ -2459,7 +2514,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="149" spans="1:4">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A149" s="1">
         <v>147</v>
       </c>
@@ -2473,7 +2528,7 @@
         <v>12.7</v>
       </c>
     </row>
-    <row r="150" spans="1:4">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A150" s="1">
         <v>148</v>
       </c>
@@ -2487,7 +2542,7 @@
         <v>13.2</v>
       </c>
     </row>
-    <row r="151" spans="1:4">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A151" s="1">
         <v>149</v>
       </c>
@@ -2501,7 +2556,7 @@
         <v>9.9</v>
       </c>
     </row>
-    <row r="152" spans="1:4">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A152" s="1">
         <v>150</v>
       </c>
@@ -2512,10 +2567,10 @@
         <v>0</v>
       </c>
       <c r="D152">
-        <v>7.199999999999999</v>
-      </c>
-    </row>
-    <row r="153" spans="1:4">
+        <v>7.1999999999999993</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A153" s="1">
         <v>151</v>
       </c>
@@ -2526,10 +2581,10 @@
         <v>0</v>
       </c>
       <c r="D153">
-        <v>8.899999999999999</v>
-      </c>
-    </row>
-    <row r="154" spans="1:4">
+        <v>8.8999999999999986</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A154" s="1">
         <v>152</v>
       </c>
@@ -2543,7 +2598,7 @@
         <v>13.7</v>
       </c>
     </row>
-    <row r="155" spans="1:4">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A155" s="1">
         <v>153</v>
       </c>
@@ -2557,7 +2612,7 @@
         <v>13.5</v>
       </c>
     </row>
-    <row r="156" spans="1:4">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A156" s="1">
         <v>154</v>
       </c>
@@ -2571,7 +2626,7 @@
         <v>11.4</v>
       </c>
     </row>
-    <row r="157" spans="1:4">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A157" s="1">
         <v>155</v>
       </c>
@@ -2585,7 +2640,7 @@
         <v>11.8</v>
       </c>
     </row>
-    <row r="158" spans="1:4">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A158" s="1">
         <v>156</v>
       </c>
@@ -2599,7 +2654,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="159" spans="1:4">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A159" s="1">
         <v>157</v>
       </c>
@@ -2610,10 +2665,10 @@
         <v>1</v>
       </c>
       <c r="D159">
-        <v>7.699999999999999</v>
-      </c>
-    </row>
-    <row r="160" spans="1:4">
+        <v>7.6999999999999993</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A160" s="1">
         <v>158</v>
       </c>
@@ -2627,7 +2682,7 @@
         <v>11.6</v>
       </c>
     </row>
-    <row r="161" spans="1:4">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A161" s="1">
         <v>159</v>
       </c>
@@ -2638,10 +2693,10 @@
         <v>0</v>
       </c>
       <c r="D161">
-        <v>9.399999999999999</v>
-      </c>
-    </row>
-    <row r="162" spans="1:4">
+        <v>9.3999999999999986</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A162" s="1">
         <v>160</v>
       </c>
@@ -2652,10 +2707,10 @@
         <v>1</v>
       </c>
       <c r="D162">
-        <v>6.199999999999999</v>
-      </c>
-    </row>
-    <row r="163" spans="1:4">
+        <v>6.1999999999999993</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A163" s="1">
         <v>161</v>
       </c>
@@ -2669,7 +2724,7 @@
         <v>10.6</v>
       </c>
     </row>
-    <row r="164" spans="1:4">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A164" s="1">
         <v>162</v>
       </c>
@@ -2683,7 +2738,7 @@
         <v>10.3</v>
       </c>
     </row>
-    <row r="165" spans="1:4">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A165" s="1">
         <v>163</v>
       </c>
@@ -2697,7 +2752,7 @@
         <v>12.2</v>
       </c>
     </row>
-    <row r="166" spans="1:4">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A166" s="1">
         <v>164</v>
       </c>
@@ -2708,10 +2763,10 @@
         <v>0</v>
       </c>
       <c r="D166">
-        <v>9.299999999999997</v>
-      </c>
-    </row>
-    <row r="167" spans="1:4">
+        <v>9.2999999999999972</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A167" s="1">
         <v>165</v>
       </c>
@@ -2725,7 +2780,7 @@
         <v>9.5</v>
       </c>
     </row>
-    <row r="168" spans="1:4">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A168" s="1">
         <v>166</v>
       </c>
@@ -2739,7 +2794,7 @@
         <v>11.1</v>
       </c>
     </row>
-    <row r="169" spans="1:4">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A169" s="1">
         <v>167</v>
       </c>
@@ -2750,10 +2805,10 @@
         <v>0</v>
       </c>
       <c r="D169">
-        <v>8.099999999999998</v>
-      </c>
-    </row>
-    <row r="170" spans="1:4">
+        <v>8.0999999999999979</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A170" s="1">
         <v>168</v>
       </c>
@@ -2764,10 +2819,10 @@
         <v>1</v>
       </c>
       <c r="D170">
-        <v>7.800000000000001</v>
-      </c>
-    </row>
-    <row r="171" spans="1:4">
+        <v>7.8000000000000007</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A171" s="1">
         <v>169</v>
       </c>
@@ -2781,7 +2836,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="172" spans="1:4">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A172" s="1">
         <v>170</v>
       </c>
@@ -2795,7 +2850,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="173" spans="1:4">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A173" s="1">
         <v>171</v>
       </c>
@@ -2806,10 +2861,10 @@
         <v>0</v>
       </c>
       <c r="D173">
-        <v>6.700000000000003</v>
-      </c>
-    </row>
-    <row r="174" spans="1:4">
+        <v>6.7000000000000028</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A174" s="1">
         <v>172</v>
       </c>
@@ -2823,7 +2878,7 @@
         <v>12.9</v>
       </c>
     </row>
-    <row r="175" spans="1:4">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A175" s="1">
         <v>173</v>
       </c>
@@ -2837,7 +2892,7 @@
         <v>11.9</v>
       </c>
     </row>
-    <row r="176" spans="1:4">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A176" s="1">
         <v>174</v>
       </c>
@@ -2851,7 +2906,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="177" spans="1:4">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A177" s="1">
         <v>175</v>
       </c>
@@ -2865,7 +2920,7 @@
         <v>13.3</v>
       </c>
     </row>
-    <row r="178" spans="1:4">
+    <row r="178" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A178" s="1">
         <v>176</v>
       </c>
@@ -2876,10 +2931,10 @@
         <v>0</v>
       </c>
       <c r="D178">
-        <v>8.800000000000001</v>
-      </c>
-    </row>
-    <row r="179" spans="1:4">
+        <v>8.8000000000000007</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A179" s="1">
         <v>177</v>
       </c>
@@ -2890,10 +2945,10 @@
         <v>0</v>
       </c>
       <c r="D179">
-        <v>9.300000000000001</v>
-      </c>
-    </row>
-    <row r="180" spans="1:4">
+        <v>9.3000000000000007</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A180" s="1">
         <v>178</v>
       </c>
@@ -2904,10 +2959,10 @@
         <v>0</v>
       </c>
       <c r="D180">
-        <v>6.699999999999999</v>
-      </c>
-    </row>
-    <row r="181" spans="1:4">
+        <v>6.6999999999999993</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A181" s="1">
         <v>179</v>
       </c>
@@ -2918,10 +2973,10 @@
         <v>0</v>
       </c>
       <c r="D181">
-        <v>8.099999999999998</v>
-      </c>
-    </row>
-    <row r="182" spans="1:4">
+        <v>8.0999999999999979</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A182" s="1">
         <v>180</v>
       </c>
@@ -2932,10 +2987,10 @@
         <v>0</v>
       </c>
       <c r="D182">
-        <v>7.600000000000001</v>
-      </c>
-    </row>
-    <row r="183" spans="1:4">
+        <v>7.6000000000000014</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A183" s="1">
         <v>181</v>
       </c>
@@ -2946,10 +3001,10 @@
         <v>0</v>
       </c>
       <c r="D183">
-        <v>8.299999999999997</v>
-      </c>
-    </row>
-    <row r="184" spans="1:4">
+        <v>8.2999999999999972</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A184" s="1">
         <v>182</v>
       </c>
@@ -2960,10 +3015,10 @@
         <v>0</v>
       </c>
       <c r="D184">
-        <v>9.300000000000001</v>
-      </c>
-    </row>
-    <row r="185" spans="1:4">
+        <v>9.3000000000000007</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A185" s="1">
         <v>183</v>
       </c>
@@ -2974,10 +3029,10 @@
         <v>0</v>
       </c>
       <c r="D185">
-        <v>6.199999999999999</v>
-      </c>
-    </row>
-    <row r="186" spans="1:4">
+        <v>6.1999999999999993</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A186" s="1">
         <v>184</v>
       </c>
@@ -2991,7 +3046,7 @@
         <v>12.8</v>
       </c>
     </row>
-    <row r="187" spans="1:4">
+    <row r="187" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A187" s="1">
         <v>185</v>
       </c>
@@ -3005,7 +3060,7 @@
         <v>14.8</v>
       </c>
     </row>
-    <row r="188" spans="1:4">
+    <row r="188" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A188" s="1">
         <v>186</v>
       </c>
@@ -3019,7 +3074,7 @@
         <v>11.5</v>
       </c>
     </row>
-    <row r="189" spans="1:4">
+    <row r="189" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A189" s="1">
         <v>187</v>
       </c>
@@ -3030,10 +3085,10 @@
         <v>0</v>
       </c>
       <c r="D189">
-        <v>9.800000000000001</v>
-      </c>
-    </row>
-    <row r="190" spans="1:4">
+        <v>9.8000000000000007</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A190" s="1">
         <v>188</v>
       </c>
@@ -3044,10 +3099,10 @@
         <v>0</v>
       </c>
       <c r="D190">
-        <v>9.800000000000001</v>
-      </c>
-    </row>
-    <row r="191" spans="1:4">
+        <v>9.8000000000000007</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A191" s="1">
         <v>189</v>
       </c>
@@ -3061,7 +3116,7 @@
         <v>10.3</v>
       </c>
     </row>
-    <row r="192" spans="1:4">
+    <row r="192" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A192" s="1">
         <v>190</v>
       </c>
@@ -3075,7 +3130,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="193" spans="1:4">
+    <row r="193" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A193" s="1">
         <v>191</v>
       </c>
@@ -3086,10 +3141,10 @@
         <v>0</v>
       </c>
       <c r="D193">
-        <v>6.399999999999999</v>
-      </c>
-    </row>
-    <row r="194" spans="1:4">
+        <v>6.3999999999999986</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A194" s="1">
         <v>192</v>
       </c>
@@ -3100,10 +3155,10 @@
         <v>0</v>
       </c>
       <c r="D194">
-        <v>8.699999999999999</v>
-      </c>
-    </row>
-    <row r="195" spans="1:4">
+        <v>8.6999999999999993</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A195" s="1">
         <v>193</v>
       </c>
@@ -3114,10 +3169,10 @@
         <v>0</v>
       </c>
       <c r="D195">
-        <v>7.599999999999998</v>
-      </c>
-    </row>
-    <row r="196" spans="1:4">
+        <v>7.5999999999999979</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A196" s="1">
         <v>194</v>
       </c>
@@ -3131,7 +3186,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="197" spans="1:4">
+    <row r="197" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A197" s="1">
         <v>195</v>
       </c>
@@ -3142,10 +3197,10 @@
         <v>1</v>
       </c>
       <c r="D197">
-        <v>5.299999999999997</v>
-      </c>
-    </row>
-    <row r="198" spans="1:4">
+        <v>5.2999999999999972</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A198" s="1">
         <v>196</v>
       </c>
@@ -3156,10 +3211,10 @@
         <v>1</v>
       </c>
       <c r="D198">
-        <v>7.400000000000002</v>
-      </c>
-    </row>
-    <row r="199" spans="1:4">
+        <v>7.4000000000000021</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A199" s="1">
         <v>197</v>
       </c>
@@ -3170,10 +3225,10 @@
         <v>0</v>
       </c>
       <c r="D199">
-        <v>6.899999999999999</v>
-      </c>
-    </row>
-    <row r="200" spans="1:4">
+        <v>6.8999999999999986</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A200" s="1">
         <v>198</v>
       </c>
@@ -3184,10 +3239,10 @@
         <v>0</v>
       </c>
       <c r="D200">
-        <v>8.800000000000001</v>
-      </c>
-    </row>
-    <row r="201" spans="1:4">
+        <v>8.8000000000000007</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A201" s="1">
         <v>199</v>
       </c>
@@ -3201,7 +3256,7 @@
         <v>12.2</v>
       </c>
     </row>
-    <row r="202" spans="1:4">
+    <row r="202" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A202" s="1">
         <v>200</v>
       </c>
@@ -3212,10 +3267,10 @@
         <v>0</v>
       </c>
       <c r="D202">
-        <v>6.799999999999997</v>
-      </c>
-    </row>
-    <row r="203" spans="1:4">
+        <v>6.7999999999999972</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A203" s="1">
         <v>201</v>
       </c>
@@ -3226,10 +3281,10 @@
         <v>1</v>
       </c>
       <c r="D203">
-        <v>2.800000000000001</v>
-      </c>
-    </row>
-    <row r="204" spans="1:4">
+        <v>2.8000000000000012</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A204" s="1">
         <v>202</v>
       </c>
@@ -3240,10 +3295,10 @@
         <v>0</v>
       </c>
       <c r="D204">
-        <v>6.800000000000001</v>
-      </c>
-    </row>
-    <row r="205" spans="1:4">
+        <v>6.8000000000000007</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A205" s="1">
         <v>203</v>
       </c>
@@ -3257,7 +3312,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="206" spans="1:4">
+    <row r="206" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A206" s="1">
         <v>204</v>
       </c>
@@ -3271,7 +3326,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="207" spans="1:4">
+    <row r="207" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A207" s="1">
         <v>205</v>
       </c>
@@ -3282,10 +3337,10 @@
         <v>1</v>
       </c>
       <c r="D207">
-        <v>1.799999999999997</v>
-      </c>
-    </row>
-    <row r="208" spans="1:4">
+        <v>1.7999999999999969</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A208" s="1">
         <v>206</v>
       </c>
@@ -3296,10 +3351,10 @@
         <v>1</v>
       </c>
       <c r="D208">
-        <v>2.199999999999999</v>
-      </c>
-    </row>
-    <row r="209" spans="1:4">
+        <v>2.1999999999999988</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A209" s="1">
         <v>207</v>
       </c>
@@ -3313,7 +3368,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="210" spans="1:4">
+    <row r="210" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A210" s="1">
         <v>208</v>
       </c>
@@ -3324,10 +3379,10 @@
         <v>1</v>
       </c>
       <c r="D210">
-        <v>3.199999999999999</v>
-      </c>
-    </row>
-    <row r="211" spans="1:4">
+        <v>3.1999999999999988</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A211" s="1">
         <v>209</v>
       </c>
@@ -3338,10 +3393,10 @@
         <v>0</v>
       </c>
       <c r="D211">
-        <v>4.399999999999999</v>
-      </c>
-    </row>
-    <row r="212" spans="1:4">
+        <v>4.3999999999999986</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A212" s="1">
         <v>210</v>
       </c>
@@ -3355,7 +3410,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="213" spans="1:4">
+    <row r="213" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A213" s="1">
         <v>211</v>
       </c>
@@ -3369,7 +3424,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="214" spans="1:4">
+    <row r="214" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A214" s="1">
         <v>212</v>
       </c>
@@ -3380,10 +3435,10 @@
         <v>1</v>
       </c>
       <c r="D214">
-        <v>6.600000000000001</v>
-      </c>
-    </row>
-    <row r="215" spans="1:4">
+        <v>6.6000000000000014</v>
+      </c>
+    </row>
+    <row r="215" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A215" s="1">
         <v>213</v>
       </c>
@@ -3394,10 +3449,10 @@
         <v>0</v>
       </c>
       <c r="D215">
-        <v>8.400000000000002</v>
-      </c>
-    </row>
-    <row r="216" spans="1:4">
+        <v>8.4000000000000021</v>
+      </c>
+    </row>
+    <row r="216" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A216" s="1">
         <v>214</v>
       </c>
@@ -3411,7 +3466,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="217" spans="1:4">
+    <row r="217" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A217" s="1">
         <v>215</v>
       </c>
@@ -3422,10 +3477,10 @@
         <v>1</v>
       </c>
       <c r="D217">
-        <v>9.399999999999999</v>
-      </c>
-    </row>
-    <row r="218" spans="1:4">
+        <v>9.3999999999999986</v>
+      </c>
+    </row>
+    <row r="218" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A218" s="1">
         <v>216</v>
       </c>
@@ -3439,7 +3494,7 @@
         <v>10.3</v>
       </c>
     </row>
-    <row r="219" spans="1:4">
+    <row r="219" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A219" s="1">
         <v>217</v>
       </c>
@@ -3450,10 +3505,10 @@
         <v>0</v>
       </c>
       <c r="D219">
-        <v>8.899999999999999</v>
-      </c>
-    </row>
-    <row r="220" spans="1:4">
+        <v>8.8999999999999986</v>
+      </c>
+    </row>
+    <row r="220" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A220" s="1">
         <v>218</v>
       </c>
@@ -3464,10 +3519,10 @@
         <v>1</v>
       </c>
       <c r="D220">
-        <v>6.400000000000002</v>
-      </c>
-    </row>
-    <row r="221" spans="1:4">
+        <v>6.4000000000000021</v>
+      </c>
+    </row>
+    <row r="221" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A221" s="1">
         <v>219</v>
       </c>
@@ -3478,10 +3533,10 @@
         <v>0</v>
       </c>
       <c r="D221">
-        <v>6.800000000000004</v>
-      </c>
-    </row>
-    <row r="222" spans="1:4">
+        <v>6.8000000000000043</v>
+      </c>
+    </row>
+    <row r="222" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A222" s="1">
         <v>220</v>
       </c>
@@ -3492,10 +3547,10 @@
         <v>0</v>
       </c>
       <c r="D222">
-        <v>8.600000000000001</v>
-      </c>
-    </row>
-    <row r="223" spans="1:4">
+        <v>8.6000000000000014</v>
+      </c>
+    </row>
+    <row r="223" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A223" s="1">
         <v>221</v>
       </c>
@@ -3506,10 +3561,10 @@
         <v>0</v>
       </c>
       <c r="D223">
-        <v>9.899999999999999</v>
-      </c>
-    </row>
-    <row r="224" spans="1:4">
+        <v>9.8999999999999986</v>
+      </c>
+    </row>
+    <row r="224" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A224" s="1">
         <v>222</v>
       </c>
@@ -3520,10 +3575,10 @@
         <v>1</v>
       </c>
       <c r="D224">
-        <v>9.400000000000002</v>
-      </c>
-    </row>
-    <row r="225" spans="1:4">
+        <v>9.4000000000000021</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A225" s="1">
         <v>223</v>
       </c>
@@ -3534,10 +3589,10 @@
         <v>1</v>
       </c>
       <c r="D225">
-        <v>3.699999999999999</v>
-      </c>
-    </row>
-    <row r="226" spans="1:4">
+        <v>3.6999999999999988</v>
+      </c>
+    </row>
+    <row r="226" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A226" s="1">
         <v>224</v>
       </c>
@@ -3548,10 +3603,10 @@
         <v>1</v>
       </c>
       <c r="D226">
-        <v>10.2</v>
-      </c>
-    </row>
-    <row r="227" spans="1:4">
+        <v>10.199999999999999</v>
+      </c>
+    </row>
+    <row r="227" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A227" s="1">
         <v>225</v>
       </c>
@@ -3562,10 +3617,10 @@
         <v>0</v>
       </c>
       <c r="D227">
-        <v>9.800000000000004</v>
-      </c>
-    </row>
-    <row r="228" spans="1:4">
+        <v>9.8000000000000043</v>
+      </c>
+    </row>
+    <row r="228" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A228" s="1">
         <v>226</v>
       </c>
@@ -3576,10 +3631,10 @@
         <v>1</v>
       </c>
       <c r="D228">
-        <v>4.700000000000003</v>
-      </c>
-    </row>
-    <row r="229" spans="1:4">
+        <v>4.7000000000000028</v>
+      </c>
+    </row>
+    <row r="229" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A229" s="1">
         <v>227</v>
       </c>
@@ -3593,7 +3648,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="230" spans="1:4">
+    <row r="230" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A230" s="1">
         <v>228</v>
       </c>
@@ -3604,10 +3659,10 @@
         <v>0</v>
       </c>
       <c r="D230">
-        <v>5.400000000000002</v>
-      </c>
-    </row>
-    <row r="231" spans="1:4">
+        <v>5.4000000000000021</v>
+      </c>
+    </row>
+    <row r="231" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A231" s="1">
         <v>229</v>
       </c>
@@ -3618,10 +3673,10 @@
         <v>0</v>
       </c>
       <c r="D231">
-        <v>8.099999999999998</v>
-      </c>
-    </row>
-    <row r="232" spans="1:4">
+        <v>8.0999999999999979</v>
+      </c>
+    </row>
+    <row r="232" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A232" s="1">
         <v>230</v>
       </c>
@@ -3635,7 +3690,7 @@
         <v>10.1</v>
       </c>
     </row>
-    <row r="233" spans="1:4">
+    <row r="233" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A233" s="1">
         <v>231</v>
       </c>
@@ -3646,10 +3701,10 @@
         <v>0</v>
       </c>
       <c r="D233">
-        <v>9.599999999999998</v>
-      </c>
-    </row>
-    <row r="234" spans="1:4">
+        <v>9.5999999999999979</v>
+      </c>
+    </row>
+    <row r="234" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A234" s="1">
         <v>232</v>
       </c>
@@ -3663,7 +3718,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="235" spans="1:4">
+    <row r="235" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A235" s="1">
         <v>233</v>
       </c>
@@ -3674,10 +3729,10 @@
         <v>0</v>
       </c>
       <c r="D235">
-        <v>8.399999999999999</v>
-      </c>
-    </row>
-    <row r="236" spans="1:4">
+        <v>8.3999999999999986</v>
+      </c>
+    </row>
+    <row r="236" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A236" s="1">
         <v>234</v>
       </c>
@@ -3688,10 +3743,10 @@
         <v>0</v>
       </c>
       <c r="D236">
-        <v>7.800000000000001</v>
-      </c>
-    </row>
-    <row r="237" spans="1:4">
+        <v>7.8000000000000007</v>
+      </c>
+    </row>
+    <row r="237" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A237" s="1">
         <v>235</v>
       </c>
@@ -3702,10 +3757,10 @@
         <v>0</v>
       </c>
       <c r="D237">
-        <v>5.800000000000001</v>
-      </c>
-    </row>
-    <row r="238" spans="1:4">
+        <v>5.8000000000000007</v>
+      </c>
+    </row>
+    <row r="238" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A238" s="1">
         <v>236</v>
       </c>
@@ -3716,10 +3771,10 @@
         <v>0</v>
       </c>
       <c r="D238">
-        <v>9.699999999999999</v>
-      </c>
-    </row>
-    <row r="239" spans="1:4">
+        <v>9.6999999999999993</v>
+      </c>
+    </row>
+    <row r="239" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A239" s="1">
         <v>237</v>
       </c>
@@ -3733,7 +3788,7 @@
         <v>10.6</v>
       </c>
     </row>
-    <row r="240" spans="1:4">
+    <row r="240" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A240" s="1">
         <v>238</v>
       </c>
@@ -3744,10 +3799,10 @@
         <v>1</v>
       </c>
       <c r="D240">
-        <v>7.100000000000001</v>
-      </c>
-    </row>
-    <row r="241" spans="1:4">
+        <v>7.1000000000000014</v>
+      </c>
+    </row>
+    <row r="241" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A241" s="1">
         <v>239</v>
       </c>
@@ -3758,10 +3813,10 @@
         <v>0</v>
       </c>
       <c r="D241">
-        <v>6.599999999999998</v>
-      </c>
-    </row>
-    <row r="242" spans="1:4">
+        <v>6.5999999999999979</v>
+      </c>
+    </row>
+    <row r="242" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A242" s="1">
         <v>240</v>
       </c>
@@ -3772,10 +3827,10 @@
         <v>1</v>
       </c>
       <c r="D242">
-        <v>6.299999999999997</v>
-      </c>
-    </row>
-    <row r="243" spans="1:4">
+        <v>6.2999999999999972</v>
+      </c>
+    </row>
+    <row r="243" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A243" s="1">
         <v>241</v>
       </c>
@@ -3789,7 +3844,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="244" spans="1:4">
+    <row r="244" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A244" s="1">
         <v>242</v>
       </c>
@@ -3803,7 +3858,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="245" spans="1:4">
+    <row r="245" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A245" s="1">
         <v>243</v>
       </c>
@@ -3814,10 +3869,10 @@
         <v>0</v>
       </c>
       <c r="D245">
-        <v>8.600000000000001</v>
-      </c>
-    </row>
-    <row r="246" spans="1:4">
+        <v>8.6000000000000014</v>
+      </c>
+    </row>
+    <row r="246" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A246" s="1">
         <v>244</v>
       </c>
@@ -3831,7 +3886,7 @@
         <v>10.3</v>
       </c>
     </row>
-    <row r="247" spans="1:4">
+    <row r="247" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A247" s="1">
         <v>245</v>
       </c>
@@ -3845,7 +3900,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="248" spans="1:4">
+    <row r="248" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A248" s="1">
         <v>246</v>
       </c>
@@ -3856,10 +3911,10 @@
         <v>1</v>
       </c>
       <c r="D248">
-        <v>4.300000000000001</v>
-      </c>
-    </row>
-    <row r="249" spans="1:4">
+        <v>4.3000000000000007</v>
+      </c>
+    </row>
+    <row r="249" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A249" s="1">
         <v>247</v>
       </c>
@@ -3870,10 +3925,10 @@
         <v>1</v>
       </c>
       <c r="D249">
-        <v>6.100000000000001</v>
-      </c>
-    </row>
-    <row r="250" spans="1:4">
+        <v>6.1000000000000014</v>
+      </c>
+    </row>
+    <row r="250" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A250" s="1">
         <v>248</v>
       </c>
@@ -3887,7 +3942,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="251" spans="1:4">
+    <row r="251" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A251" s="1">
         <v>249</v>
       </c>
@@ -3898,10 +3953,10 @@
         <v>0</v>
       </c>
       <c r="D251">
-        <v>6.899999999999999</v>
-      </c>
-    </row>
-    <row r="252" spans="1:4">
+        <v>6.8999999999999986</v>
+      </c>
+    </row>
+    <row r="252" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A252" s="1">
         <v>250</v>
       </c>
@@ -3912,10 +3967,10 @@
         <v>0</v>
       </c>
       <c r="D252">
-        <v>4.400000000000002</v>
-      </c>
-    </row>
-    <row r="253" spans="1:4">
+        <v>4.4000000000000021</v>
+      </c>
+    </row>
+    <row r="253" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A253" s="1">
         <v>251</v>
       </c>
@@ -3926,10 +3981,10 @@
         <v>0</v>
       </c>
       <c r="D253">
-        <v>5.600000000000001</v>
-      </c>
-    </row>
-    <row r="254" spans="1:4">
+        <v>5.6000000000000014</v>
+      </c>
+    </row>
+    <row r="254" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A254" s="1">
         <v>252</v>
       </c>
@@ -3940,10 +3995,10 @@
         <v>1</v>
       </c>
       <c r="D254">
-        <v>4.399999999999999</v>
-      </c>
-    </row>
-    <row r="255" spans="1:4">
+        <v>4.3999999999999986</v>
+      </c>
+    </row>
+    <row r="255" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A255" s="1">
         <v>253</v>
       </c>
@@ -3954,10 +4009,10 @@
         <v>1</v>
       </c>
       <c r="D255">
-        <v>8.300000000000001</v>
-      </c>
-    </row>
-    <row r="256" spans="1:4">
+        <v>8.3000000000000007</v>
+      </c>
+    </row>
+    <row r="256" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A256" s="1">
         <v>254</v>
       </c>
@@ -3968,10 +4023,10 @@
         <v>0</v>
       </c>
       <c r="D256">
-        <v>4.199999999999999</v>
-      </c>
-    </row>
-    <row r="257" spans="1:4">
+        <v>4.1999999999999993</v>
+      </c>
+    </row>
+    <row r="257" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A257" s="1">
         <v>255</v>
       </c>
@@ -3985,7 +4040,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="258" spans="1:4">
+    <row r="258" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A258" s="1">
         <v>256</v>
       </c>
@@ -3996,10 +4051,10 @@
         <v>0</v>
       </c>
       <c r="D258">
-        <v>3.300000000000001</v>
-      </c>
-    </row>
-    <row r="259" spans="1:4">
+        <v>3.3000000000000012</v>
+      </c>
+    </row>
+    <row r="259" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A259" s="1">
         <v>257</v>
       </c>
@@ -4013,7 +4068,7 @@
         <v>10.5</v>
       </c>
     </row>
-    <row r="260" spans="1:4">
+    <row r="260" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A260" s="1">
         <v>258</v>
       </c>
@@ -4024,10 +4079,10 @@
         <v>0</v>
       </c>
       <c r="D260">
-        <v>9.800000000000001</v>
-      </c>
-    </row>
-    <row r="261" spans="1:4">
+        <v>9.8000000000000007</v>
+      </c>
+    </row>
+    <row r="261" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A261" s="1">
         <v>259</v>
       </c>
@@ -4041,7 +4096,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="262" spans="1:4">
+    <row r="262" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A262" s="1">
         <v>260</v>
       </c>
@@ -4052,10 +4107,10 @@
         <v>0</v>
       </c>
       <c r="D262">
-        <v>9.399999999999999</v>
-      </c>
-    </row>
-    <row r="263" spans="1:4">
+        <v>9.3999999999999986</v>
+      </c>
+    </row>
+    <row r="263" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A263" s="1">
         <v>261</v>
       </c>
@@ -4069,7 +4124,7 @@
         <v>12.4</v>
       </c>
     </row>
-    <row r="264" spans="1:4">
+    <row r="264" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A264" s="1">
         <v>262</v>
       </c>
@@ -4080,10 +4135,10 @@
         <v>0</v>
       </c>
       <c r="D264">
-        <v>8.399999999999999</v>
-      </c>
-    </row>
-    <row r="265" spans="1:4">
+        <v>8.3999999999999986</v>
+      </c>
+    </row>
+    <row r="265" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A265" s="1">
         <v>263</v>
       </c>
@@ -4094,10 +4149,10 @@
         <v>0</v>
       </c>
       <c r="D265">
-        <v>3.800000000000001</v>
-      </c>
-    </row>
-    <row r="266" spans="1:4">
+        <v>3.8000000000000012</v>
+      </c>
+    </row>
+    <row r="266" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A266" s="1">
         <v>264</v>
       </c>
@@ -4108,10 +4163,10 @@
         <v>0</v>
       </c>
       <c r="D266">
-        <v>2.300000000000001</v>
-      </c>
-    </row>
-    <row r="267" spans="1:4">
+        <v>2.3000000000000012</v>
+      </c>
+    </row>
+    <row r="267" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A267" s="1">
         <v>265</v>
       </c>
@@ -4122,10 +4177,10 @@
         <v>0</v>
       </c>
       <c r="D267">
-        <v>7.700000000000003</v>
-      </c>
-    </row>
-    <row r="268" spans="1:4">
+        <v>7.7000000000000028</v>
+      </c>
+    </row>
+    <row r="268" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A268" s="1">
         <v>266</v>
       </c>
@@ -4139,7 +4194,7 @@
         <v>12.6</v>
       </c>
     </row>
-    <row r="269" spans="1:4">
+    <row r="269" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A269" s="1">
         <v>267</v>
       </c>
@@ -4153,7 +4208,7 @@
         <v>12.6</v>
       </c>
     </row>
-    <row r="270" spans="1:4">
+    <row r="270" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A270" s="1">
         <v>268</v>
       </c>
@@ -4167,7 +4222,7 @@
         <v>11.3</v>
       </c>
     </row>
-    <row r="271" spans="1:4">
+    <row r="271" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A271" s="1">
         <v>269</v>
       </c>
@@ -4178,10 +4233,10 @@
         <v>0</v>
       </c>
       <c r="D271">
-        <v>7.399999999999999</v>
-      </c>
-    </row>
-    <row r="272" spans="1:4">
+        <v>7.3999999999999986</v>
+      </c>
+    </row>
+    <row r="272" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A272" s="1">
         <v>270</v>
       </c>
@@ -4192,10 +4247,10 @@
         <v>0</v>
       </c>
       <c r="D272">
-        <v>9.800000000000001</v>
-      </c>
-    </row>
-    <row r="273" spans="1:4">
+        <v>9.8000000000000007</v>
+      </c>
+    </row>
+    <row r="273" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A273" s="1">
         <v>271</v>
       </c>
@@ -4209,7 +4264,7 @@
         <v>10.7</v>
       </c>
     </row>
-    <row r="274" spans="1:4">
+    <row r="274" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A274" s="1">
         <v>272</v>
       </c>
@@ -4223,7 +4278,7 @@
         <v>13.5</v>
       </c>
     </row>
-    <row r="275" spans="1:4">
+    <row r="275" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A275" s="1">
         <v>273</v>
       </c>
@@ -4237,7 +4292,7 @@
         <v>10.6</v>
       </c>
     </row>
-    <row r="276" spans="1:4">
+    <row r="276" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A276" s="1">
         <v>274</v>
       </c>
@@ -4248,10 +4303,10 @@
         <v>1</v>
       </c>
       <c r="D276">
-        <v>4.199999999999999</v>
-      </c>
-    </row>
-    <row r="277" spans="1:4">
+        <v>4.1999999999999993</v>
+      </c>
+    </row>
+    <row r="277" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A277" s="1">
         <v>275</v>
       </c>
@@ -4265,7 +4320,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="278" spans="1:4">
+    <row r="278" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A278" s="1">
         <v>276</v>
       </c>
@@ -4276,10 +4331,10 @@
         <v>0</v>
       </c>
       <c r="D278">
-        <v>9.800000000000001</v>
-      </c>
-    </row>
-    <row r="279" spans="1:4">
+        <v>9.8000000000000007</v>
+      </c>
+    </row>
+    <row r="279" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A279" s="1">
         <v>277</v>
       </c>
@@ -4290,10 +4345,10 @@
         <v>0</v>
       </c>
       <c r="D279">
-        <v>7.199999999999999</v>
-      </c>
-    </row>
-    <row r="280" spans="1:4">
+        <v>7.1999999999999993</v>
+      </c>
+    </row>
+    <row r="280" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A280" s="1">
         <v>278</v>
       </c>
@@ -4307,7 +4362,7 @@
         <v>9.5</v>
       </c>
     </row>
-    <row r="281" spans="1:4">
+    <row r="281" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A281" s="1">
         <v>279</v>
       </c>
@@ -4318,10 +4373,10 @@
         <v>1</v>
       </c>
       <c r="D281">
-        <v>4.599999999999998</v>
-      </c>
-    </row>
-    <row r="282" spans="1:4">
+        <v>4.5999999999999979</v>
+      </c>
+    </row>
+    <row r="282" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A282" s="1">
         <v>280</v>
       </c>
@@ -4332,10 +4387,10 @@
         <v>0</v>
       </c>
       <c r="D282">
-        <v>9.200000000000001</v>
-      </c>
-    </row>
-    <row r="283" spans="1:4">
+        <v>9.2000000000000011</v>
+      </c>
+    </row>
+    <row r="283" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A283" s="1">
         <v>281</v>
       </c>
@@ -4349,7 +4404,7 @@
         <v>12.7</v>
       </c>
     </row>
-    <row r="284" spans="1:4">
+    <row r="284" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A284" s="1">
         <v>282</v>
       </c>
@@ -4360,10 +4415,10 @@
         <v>0</v>
       </c>
       <c r="D284">
-        <v>9.100000000000001</v>
-      </c>
-    </row>
-    <row r="285" spans="1:4">
+        <v>9.1000000000000014</v>
+      </c>
+    </row>
+    <row r="285" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A285" s="1">
         <v>283</v>
       </c>
@@ -4377,7 +4432,7 @@
         <v>13.1</v>
       </c>
     </row>
-    <row r="286" spans="1:4">
+    <row r="286" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A286" s="1">
         <v>284</v>
       </c>
@@ -4391,7 +4446,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="287" spans="1:4">
+    <row r="287" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A287" s="1">
         <v>285</v>
       </c>
@@ -4405,7 +4460,7 @@
         <v>11.7</v>
       </c>
     </row>
-    <row r="288" spans="1:4">
+    <row r="288" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A288" s="1">
         <v>286</v>
       </c>
@@ -4419,7 +4474,7 @@
         <v>10.1</v>
       </c>
     </row>
-    <row r="289" spans="1:4">
+    <row r="289" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A289" s="1">
         <v>287</v>
       </c>
@@ -4433,7 +4488,7 @@
         <v>11.6</v>
       </c>
     </row>
-    <row r="290" spans="1:4">
+    <row r="290" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A290" s="1">
         <v>288</v>
       </c>
@@ -4447,7 +4502,7 @@
         <v>11.8</v>
       </c>
     </row>
-    <row r="291" spans="1:4">
+    <row r="291" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A291" s="1">
         <v>289</v>
       </c>
@@ -4461,7 +4516,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="292" spans="1:4">
+    <row r="292" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A292" s="1">
         <v>290</v>
       </c>
@@ -4475,7 +4530,7 @@
         <v>10.7</v>
       </c>
     </row>
-    <row r="293" spans="1:4">
+    <row r="293" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A293" s="1">
         <v>291</v>
       </c>
@@ -4489,7 +4544,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="294" spans="1:4">
+    <row r="294" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A294" s="1">
         <v>292</v>
       </c>
@@ -4503,7 +4558,7 @@
         <v>10.9</v>
       </c>
     </row>
-    <row r="295" spans="1:4">
+    <row r="295" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A295" s="1">
         <v>293</v>
       </c>
@@ -4517,7 +4572,7 @@
         <v>13.7</v>
       </c>
     </row>
-    <row r="296" spans="1:4">
+    <row r="296" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A296" s="1">
         <v>294</v>
       </c>
@@ -4531,7 +4586,7 @@
         <v>11.1</v>
       </c>
     </row>
-    <row r="297" spans="1:4">
+    <row r="297" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A297" s="1">
         <v>295</v>
       </c>
@@ -4542,10 +4597,10 @@
         <v>0</v>
       </c>
       <c r="D297">
-        <v>6.399999999999999</v>
-      </c>
-    </row>
-    <row r="298" spans="1:4">
+        <v>6.3999999999999986</v>
+      </c>
+    </row>
+    <row r="298" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A298" s="1">
         <v>296</v>
       </c>
@@ -4559,7 +4614,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="299" spans="1:4">
+    <row r="299" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A299" s="1">
         <v>297</v>
       </c>
@@ -4573,7 +4628,7 @@
         <v>8.9</v>
       </c>
     </row>
-    <row r="300" spans="1:4">
+    <row r="300" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A300" s="1">
         <v>298</v>
       </c>
@@ -4584,10 +4639,10 @@
         <v>0</v>
       </c>
       <c r="D300">
-        <v>8.300000000000001</v>
-      </c>
-    </row>
-    <row r="301" spans="1:4">
+        <v>8.3000000000000007</v>
+      </c>
+    </row>
+    <row r="301" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A301" s="1">
         <v>299</v>
       </c>
@@ -4601,7 +4656,7 @@
         <v>12.7</v>
       </c>
     </row>
-    <row r="302" spans="1:4">
+    <row r="302" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A302" s="1">
         <v>300</v>
       </c>
@@ -4615,7 +4670,7 @@
         <v>10.3</v>
       </c>
     </row>
-    <row r="303" spans="1:4">
+    <row r="303" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A303" s="1">
         <v>301</v>
       </c>
@@ -4626,10 +4681,10 @@
         <v>0</v>
       </c>
       <c r="D303">
-        <v>9.400000000000002</v>
-      </c>
-    </row>
-    <row r="304" spans="1:4">
+        <v>9.4000000000000021</v>
+      </c>
+    </row>
+    <row r="304" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A304" s="1">
         <v>302</v>
       </c>
@@ -4643,7 +4698,7 @@
         <v>12.7</v>
       </c>
     </row>
-    <row r="305" spans="1:4">
+    <row r="305" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A305" s="1">
         <v>303</v>
       </c>
@@ -4657,7 +4712,7 @@
         <v>11.3</v>
       </c>
     </row>
-    <row r="306" spans="1:4">
+    <row r="306" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A306" s="1">
         <v>304</v>
       </c>
@@ -4671,7 +4726,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="307" spans="1:4">
+    <row r="307" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A307" s="1">
         <v>305</v>
       </c>
@@ -4685,7 +4740,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="308" spans="1:4">
+    <row r="308" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A308" s="1">
         <v>306</v>
       </c>
@@ -4699,7 +4754,7 @@
         <v>12.7</v>
       </c>
     </row>
-    <row r="309" spans="1:4">
+    <row r="309" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A309" s="1">
         <v>307</v>
       </c>
@@ -4713,7 +4768,7 @@
         <v>11.1</v>
       </c>
     </row>
-    <row r="310" spans="1:4">
+    <row r="310" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A310" s="1">
         <v>308</v>
       </c>
@@ -4724,10 +4779,10 @@
         <v>0</v>
       </c>
       <c r="D310">
-        <v>9.999999999999998</v>
-      </c>
-    </row>
-    <row r="311" spans="1:4">
+        <v>9.9999999999999982</v>
+      </c>
+    </row>
+    <row r="311" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A311" s="1">
         <v>309</v>
       </c>
@@ -4738,10 +4793,10 @@
         <v>0</v>
       </c>
       <c r="D311">
-        <v>10.2</v>
-      </c>
-    </row>
-    <row r="312" spans="1:4">
+        <v>10.199999999999999</v>
+      </c>
+    </row>
+    <row r="312" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A312" s="1">
         <v>310</v>
       </c>
@@ -4755,7 +4810,7 @@
         <v>8.6</v>
       </c>
     </row>
-    <row r="313" spans="1:4">
+    <row r="313" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A313" s="1">
         <v>311</v>
       </c>
@@ -4769,7 +4824,7 @@
         <v>11.9</v>
       </c>
     </row>
-    <row r="314" spans="1:4">
+    <row r="314" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A314" s="1">
         <v>312</v>
       </c>
@@ -4783,7 +4838,7 @@
         <v>13.7</v>
       </c>
     </row>
-    <row r="315" spans="1:4">
+    <row r="315" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A315" s="1">
         <v>313</v>
       </c>
@@ -4794,10 +4849,10 @@
         <v>1</v>
       </c>
       <c r="D315">
-        <v>9.100000000000001</v>
-      </c>
-    </row>
-    <row r="316" spans="1:4">
+        <v>9.1000000000000014</v>
+      </c>
+    </row>
+    <row r="316" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A316" s="1">
         <v>314</v>
       </c>
@@ -4808,10 +4863,10 @@
         <v>0</v>
       </c>
       <c r="D316">
-        <v>7.199999999999999</v>
-      </c>
-    </row>
-    <row r="317" spans="1:4">
+        <v>7.1999999999999993</v>
+      </c>
+    </row>
+    <row r="317" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A317" s="1">
         <v>315</v>
       </c>
@@ -4822,10 +4877,10 @@
         <v>0</v>
       </c>
       <c r="D317">
-        <v>9.699999999999999</v>
-      </c>
-    </row>
-    <row r="318" spans="1:4">
+        <v>9.6999999999999993</v>
+      </c>
+    </row>
+    <row r="318" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A318" s="1">
         <v>316</v>
       </c>
@@ -4836,10 +4891,10 @@
         <v>1</v>
       </c>
       <c r="D318">
-        <v>8.300000000000001</v>
-      </c>
-    </row>
-    <row r="319" spans="1:4">
+        <v>8.3000000000000007</v>
+      </c>
+    </row>
+    <row r="319" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A319" s="1">
         <v>317</v>
       </c>
@@ -4853,7 +4908,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="320" spans="1:4">
+    <row r="320" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A320" s="1">
         <v>318</v>
       </c>
@@ -4864,10 +4919,10 @@
         <v>1</v>
       </c>
       <c r="D320">
-        <v>6.199999999999999</v>
-      </c>
-    </row>
-    <row r="321" spans="1:4">
+        <v>6.1999999999999993</v>
+      </c>
+    </row>
+    <row r="321" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A321" s="1">
         <v>319</v>
       </c>
@@ -4878,10 +4933,10 @@
         <v>0</v>
       </c>
       <c r="D321">
-        <v>8.899999999999999</v>
-      </c>
-    </row>
-    <row r="322" spans="1:4">
+        <v>8.8999999999999986</v>
+      </c>
+    </row>
+    <row r="322" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A322" s="1">
         <v>320</v>
       </c>
@@ -4892,10 +4947,10 @@
         <v>1</v>
       </c>
       <c r="D322">
-        <v>4.9</v>
-      </c>
-    </row>
-    <row r="323" spans="1:4">
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="323" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A323" s="1">
         <v>321</v>
       </c>
@@ -4909,7 +4964,7 @@
         <v>12.3</v>
       </c>
     </row>
-    <row r="324" spans="1:4">
+    <row r="324" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A324" s="1">
         <v>322</v>
       </c>
@@ -4923,7 +4978,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="325" spans="1:4">
+    <row r="325" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A325" s="1">
         <v>323</v>
       </c>
@@ -4937,7 +4992,7 @@
         <v>10.9</v>
       </c>
     </row>
-    <row r="326" spans="1:4">
+    <row r="326" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A326" s="1">
         <v>324</v>
       </c>
@@ -4951,7 +5006,7 @@
         <v>11.3</v>
       </c>
     </row>
-    <row r="327" spans="1:4">
+    <row r="327" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A327" s="1">
         <v>325</v>
       </c>
@@ -4965,7 +5020,7 @@
         <v>14.3</v>
       </c>
     </row>
-    <row r="328" spans="1:4">
+    <row r="328" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A328" s="1">
         <v>326</v>
       </c>
@@ -4979,7 +5034,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="329" spans="1:4">
+    <row r="329" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A329" s="1">
         <v>327</v>
       </c>
@@ -4993,7 +5048,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="330" spans="1:4">
+    <row r="330" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A330" s="1">
         <v>328</v>
       </c>
@@ -5007,7 +5062,7 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="331" spans="1:4">
+    <row r="331" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A331" s="1">
         <v>329</v>
       </c>
@@ -5021,7 +5076,7 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="332" spans="1:4">
+    <row r="332" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A332" s="1">
         <v>330</v>
       </c>
@@ -5035,7 +5090,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="333" spans="1:4">
+    <row r="333" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A333" s="1">
         <v>331</v>
       </c>
@@ -5049,7 +5104,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="334" spans="1:4">
+    <row r="334" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A334" s="1">
         <v>332</v>
       </c>
@@ -5063,7 +5118,7 @@
         <v>10.3</v>
       </c>
     </row>
-    <row r="335" spans="1:4">
+    <row r="335" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A335" s="1">
         <v>333</v>
       </c>
@@ -5077,7 +5132,7 @@
         <v>10.7</v>
       </c>
     </row>
-    <row r="336" spans="1:4">
+    <row r="336" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A336" s="1">
         <v>334</v>
       </c>
@@ -5091,7 +5146,7 @@
         <v>3.9</v>
       </c>
     </row>
-    <row r="337" spans="1:4">
+    <row r="337" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A337" s="1">
         <v>335</v>
       </c>
@@ -5105,7 +5160,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="338" spans="1:4">
+    <row r="338" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A338" s="1">
         <v>336</v>
       </c>
@@ -5116,10 +5171,10 @@
         <v>0</v>
       </c>
       <c r="D338">
-        <v>9.199999999999999</v>
-      </c>
-    </row>
-    <row r="339" spans="1:4">
+        <v>9.1999999999999993</v>
+      </c>
+    </row>
+    <row r="339" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A339" s="1">
         <v>337</v>
       </c>
@@ -5130,10 +5185,10 @@
         <v>0</v>
       </c>
       <c r="D339">
-        <v>9.199999999999999</v>
-      </c>
-    </row>
-    <row r="340" spans="1:4">
+        <v>9.1999999999999993</v>
+      </c>
+    </row>
+    <row r="340" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A340" s="1">
         <v>338</v>
       </c>
@@ -5144,10 +5199,10 @@
         <v>0</v>
       </c>
       <c r="D340">
-        <v>8.300000000000001</v>
-      </c>
-    </row>
-    <row r="341" spans="1:4">
+        <v>8.3000000000000007</v>
+      </c>
+    </row>
+    <row r="341" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A341" s="1">
         <v>339</v>
       </c>
@@ -5161,7 +5216,7 @@
         <v>9.6</v>
       </c>
     </row>
-    <row r="342" spans="1:4">
+    <row r="342" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A342" s="1">
         <v>340</v>
       </c>
@@ -5175,7 +5230,7 @@
         <v>6.7</v>
       </c>
     </row>
-    <row r="343" spans="1:4">
+    <row r="343" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A343" s="1">
         <v>341</v>
       </c>
@@ -5189,7 +5244,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="344" spans="1:4">
+    <row r="344" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A344" s="1">
         <v>342</v>
       </c>
@@ -5200,10 +5255,10 @@
         <v>0</v>
       </c>
       <c r="D344">
-        <v>9.300000000000001</v>
-      </c>
-    </row>
-    <row r="345" spans="1:4">
+        <v>9.3000000000000007</v>
+      </c>
+    </row>
+    <row r="345" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A345" s="1">
         <v>343</v>
       </c>
@@ -5214,10 +5269,10 @@
         <v>0</v>
       </c>
       <c r="D345">
-        <v>4.800000000000001</v>
-      </c>
-    </row>
-    <row r="346" spans="1:4">
+        <v>4.8000000000000007</v>
+      </c>
+    </row>
+    <row r="346" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A346" s="1">
         <v>344</v>
       </c>
@@ -5228,10 +5283,10 @@
         <v>0</v>
       </c>
       <c r="D346">
-        <v>9.700000000000001</v>
-      </c>
-    </row>
-    <row r="347" spans="1:4">
+        <v>9.7000000000000011</v>
+      </c>
+    </row>
+    <row r="347" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A347" s="1">
         <v>345</v>
       </c>
@@ -5245,7 +5300,7 @@
         <v>6.9</v>
       </c>
     </row>
-    <row r="348" spans="1:4">
+    <row r="348" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A348" s="1">
         <v>346</v>
       </c>
@@ -5256,10 +5311,10 @@
         <v>0</v>
       </c>
       <c r="D348">
-        <v>9.600000000000001</v>
-      </c>
-    </row>
-    <row r="349" spans="1:4">
+        <v>9.6000000000000014</v>
+      </c>
+    </row>
+    <row r="349" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A349" s="1">
         <v>347</v>
       </c>
@@ -5273,7 +5328,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="350" spans="1:4">
+    <row r="350" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A350" s="1">
         <v>348</v>
       </c>
@@ -5287,7 +5342,7 @@
         <v>10.6</v>
       </c>
     </row>
-    <row r="351" spans="1:4">
+    <row r="351" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A351" s="1">
         <v>349</v>
       </c>
@@ -5301,7 +5356,7 @@
         <v>10.8</v>
       </c>
     </row>
-    <row r="352" spans="1:4">
+    <row r="352" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A352" s="1">
         <v>350</v>
       </c>
@@ -5312,10 +5367,10 @@
         <v>1</v>
       </c>
       <c r="D352">
-        <v>6.999999999999999</v>
-      </c>
-    </row>
-    <row r="353" spans="1:4">
+        <v>6.9999999999999991</v>
+      </c>
+    </row>
+    <row r="353" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A353" s="1">
         <v>351</v>
       </c>
@@ -5329,7 +5384,7 @@
         <v>6.9</v>
       </c>
     </row>
-    <row r="354" spans="1:4">
+    <row r="354" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A354" s="1">
         <v>352</v>
       </c>
@@ -5343,7 +5398,7 @@
         <v>7.6</v>
       </c>
     </row>
-    <row r="355" spans="1:4">
+    <row r="355" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A355" s="1">
         <v>353</v>
       </c>
@@ -5357,7 +5412,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="356" spans="1:4">
+    <row r="356" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A356" s="1">
         <v>354</v>
       </c>
@@ -5371,7 +5426,7 @@
         <v>6.6</v>
       </c>
     </row>
-    <row r="357" spans="1:4">
+    <row r="357" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A357" s="1">
         <v>355</v>
       </c>
@@ -5385,7 +5440,7 @@
         <v>8.1</v>
       </c>
     </row>
-    <row r="358" spans="1:4">
+    <row r="358" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A358" s="1">
         <v>356</v>
       </c>
@@ -5396,10 +5451,10 @@
         <v>0</v>
       </c>
       <c r="D358">
-        <v>4.9</v>
-      </c>
-    </row>
-    <row r="359" spans="1:4">
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="359" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A359" s="1">
         <v>357</v>
       </c>
@@ -5413,7 +5468,7 @@
         <v>9.4</v>
       </c>
     </row>
-    <row r="360" spans="1:4">
+    <row r="360" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A360" s="1">
         <v>358</v>
       </c>
@@ -5424,10 +5479,10 @@
         <v>0</v>
       </c>
       <c r="D360">
-        <v>9.300000000000001</v>
-      </c>
-    </row>
-    <row r="361" spans="1:4">
+        <v>9.3000000000000007</v>
+      </c>
+    </row>
+    <row r="361" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A361" s="1">
         <v>359</v>
       </c>
@@ -5441,7 +5496,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="362" spans="1:4">
+    <row r="362" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A362" s="1">
         <v>360</v>
       </c>
@@ -5452,10 +5507,10 @@
         <v>0</v>
       </c>
       <c r="D362">
-        <v>7.199999999999999</v>
-      </c>
-    </row>
-    <row r="363" spans="1:4">
+        <v>7.1999999999999993</v>
+      </c>
+    </row>
+    <row r="363" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A363" s="1">
         <v>361</v>
       </c>
@@ -5466,10 +5521,10 @@
         <v>0</v>
       </c>
       <c r="D363">
-        <v>9.699999999999999</v>
-      </c>
-    </row>
-    <row r="364" spans="1:4">
+        <v>9.6999999999999993</v>
+      </c>
+    </row>
+    <row r="364" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A364" s="1">
         <v>362</v>
       </c>
@@ -5480,10 +5535,10 @@
         <v>0</v>
       </c>
       <c r="D364">
-        <v>5.1</v>
-      </c>
-    </row>
-    <row r="365" spans="1:4">
+        <v>5.0999999999999996</v>
+      </c>
+    </row>
+    <row r="365" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A365" s="1">
         <v>363</v>
       </c>
@@ -5497,7 +5552,7 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="366" spans="1:4">
+    <row r="366" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A366" s="1">
         <v>364</v>
       </c>
@@ -5508,6 +5563,20 @@
         <v>0</v>
       </c>
       <c r="D366">
+        <v>6.4</v>
+      </c>
+    </row>
+    <row r="367" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A367" s="1">
+        <v>365</v>
+      </c>
+      <c r="B367" s="2">
+        <v>43831</v>
+      </c>
+      <c r="C367">
+        <v>0</v>
+      </c>
+      <c r="D367">
         <v>6.4</v>
       </c>
     </row>

</xml_diff>